<commit_message>
updates to CV with additional research information
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65E3991D-5116-0A4B-836C-D2FE27A4AAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33986FFB-01E3-EE4D-9DB4-07FEB38C50D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="27640" windowHeight="15660" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
+    <workbookView xWindow="-19860" yWindow="-18000" windowWidth="27640" windowHeight="15660" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="70">
   <si>
     <t>type</t>
   </si>
@@ -93,9 +93,6 @@
     <t>University of Illinois at Urbana-Champaign</t>
   </si>
   <si>
-    <t xml:space="preserve">Provide clinical supervison to Master's students in the Communication Disorders and Sciences program, primarily for treatment sessions in the School-Age Clinic and the Brain Injury and Concussion Clinic </t>
-  </si>
-  <si>
     <t xml:space="preserve">history </t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t xml:space="preserve">student_service </t>
   </si>
   <si>
-    <t xml:space="preserve">Data Consultant </t>
-  </si>
-  <si>
     <t xml:space="preserve">Hawaii Concussion Awareness and Management Program (HCAMP) </t>
   </si>
   <si>
@@ -156,21 +150,9 @@
     <t xml:space="preserve">Responsible for development of the clinic term schedule, recruitment of clients, development of assessment materials to measure student outcome, and the development of a treatment protocol for adolescents with prolonged concussion symptoms </t>
   </si>
   <si>
-    <t xml:space="preserve">Research Assistant </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eugene Youth Concussion Management Team </t>
-  </si>
-  <si>
-    <t>Assisted in the development of system for client data tracking and provided clinical supervision to clients treated in the BrICC</t>
-  </si>
-  <si>
     <t>Co-director, Brain Injury and Concussion Clinic (BrICC)</t>
   </si>
   <si>
-    <t>https://jim-wright90.github.io/cmt_plots/</t>
-  </si>
-  <si>
     <t>professional_affiliation</t>
   </si>
   <si>
@@ -183,9 +165,6 @@
     <t>certification_licensure</t>
   </si>
   <si>
-    <t xml:space="preserve">License in Speech-Langauge Pathology </t>
-  </si>
-  <si>
     <t>State of Oregon</t>
   </si>
   <si>
@@ -238,16 +217,51 @@
   </si>
   <si>
     <t>Course instructor for CDS 663: *Management of Acquired Cognitive Disorders*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student_research </t>
+  </si>
+  <si>
+    <t>Assisted Dr. Torrey Loucks in the collection, analysis, and interpretation of data from speech samples pertaining to the effects of delayed auditory feedback (DAF) on fluent speakers and speakers who stutter</t>
+  </si>
+  <si>
+    <t>Teaching assistant for SHS 410: *Stuttering: Theory &amp; Practice*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research assistant, NeuroSpeech Laboratory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Academic advisor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">License in Speech-Language Pathology </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provide clinical supervision to Master's students in the Communication Disorders and Sciences program, primarily for treatment sessions in the School-Age Clinic and the Brain Injury and Concussion Clinic </t>
+  </si>
+  <si>
+    <t>Advised incoming freshmen students on the selection of courses for their first term enrolled in the Department of Communication Disorders &amp; Sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data consultant </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,16 +284,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -592,9 +611,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8559F42B-99AA-F44B-B1DC-6C413C767572}">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -708,12 +727,12 @@
         <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="1">
         <v>2016</v>
@@ -722,13 +741,13 @@
         <v>2017</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -742,18 +761,18 @@
         <v>2017</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1">
         <v>2015</v>
@@ -762,13 +781,13 @@
         <v>2016</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -782,13 +801,13 @@
         <v>2015</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="136" x14ac:dyDescent="0.2">
@@ -802,115 +821,118 @@
         <v>2014</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="204" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C12" s="1">
         <v>2021</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="221" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C13" s="1">
         <v>2021</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="187" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="B14" s="1">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="C14" s="1">
+        <v>2014</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
         <v>2021</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="204" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2020</v>
       </c>
       <c r="C15" s="1">
         <v>2021</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>34</v>
+      <c r="D15" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="221" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="C16" s="1">
         <v>2021</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>2018</v>
@@ -919,143 +941,199 @@
         <v>2021</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="119" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>2014</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2014</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="221" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>2018</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2021</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="136" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B20" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>2018</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2019</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B21" s="1">
         <v>2015</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="136" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="1">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2015</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1">
         <v>2019</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="272" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="1">
+      <c r="D27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="272" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="1">
         <v>2019</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>61</v>
+      <c r="D28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{9FC96BBB-E6A2-B445-A8BC-D5C33750B0BD}"/>
+    <hyperlink ref="G15" r:id="rId2" xr:uid="{67F88AC2-2CFE-FA4A-92CE-3F4ED8A9D293}"/>
+    <hyperlink ref="D15" r:id="rId3" xr:uid="{67C34580-503B-904D-B129-0E6417699D1E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed typo and year update
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47912172-2051-B34E-BCC0-C74E0E470A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA065E2-9B77-B640-AC61-2560AD824A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
   </bookViews>
@@ -270,13 +270,13 @@
     <t xml:space="preserve">Researcher </t>
   </si>
   <si>
-    <t>Rsearch Associate</t>
-  </si>
-  <si>
     <t>Support and lead multiple aspects of research and evaluation studies and technical assistance projects via data collection, management, and analysis as well as meeting facilitation and report writing</t>
   </si>
   <si>
     <t>Support multiple aspects of research and evaluation studies designed to inform educational improvement through the provision of technical support and communication of findings</t>
+  </si>
+  <si>
+    <t>Research Associate</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,7 +760,7 @@
         <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="170" x14ac:dyDescent="0.2">
@@ -771,16 +771,16 @@
         <v>2022</v>
       </c>
       <c r="C7" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="170" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
trying to fix render error
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCB097B-806B-754D-985A-1618D093FE10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53B60CD-DA88-E74D-9B4C-CEF3B1C4B414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
   </bookViews>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8559F42B-99AA-F44B-B1DC-6C413C767572}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates for May 2025 application
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/Resume/wright_cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898A46CE-AE36-F348-8968-237590554C75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D23AADE-F79F-2C4A-B901-BF42EB2D0FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25780" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{C4D43CE4-6AA2-144D-A346-CE8B2E756935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="128">
   <si>
     <t>type</t>
   </si>
@@ -400,6 +400,24 @@
   </si>
   <si>
     <t xml:space="preserve">Translate high-level project goals into actionable work plans, ensuring that every phase moves forward smoothly and on schedule. Oversee project implementation, anticipating resource needs, troubleshooting challenges, and making strategic adjustments when necessary. Manage relationships with partners and stakeholders, ensuring their needs are met through clear communication and collaboration. Delegate effectively, solve problems proactively, and keep projects on track from start to finish. Focus on maintaining momentum, driving results, and continuously improving processes to deliver successful outcomes. </t>
+  </si>
+  <si>
+    <t>Lake, Kern, Siskiyou, Sutter, Yuba, and Ventura Counties, CA</t>
+  </si>
+  <si>
+    <t>Butte, Plumas, and Santa Cruz County Offices of Education, CA</t>
+  </si>
+  <si>
+    <t>Lead Project Manager for ASR's consulting work with six California First 5 County Commissions. Support Commission efforts related to annual program evaluation, including data collection, management, analysis, and reporting. Facilitate strategic planning initiatives, including the design and distribution of surveys via Qualtrics and the collection of qualitative data through focus groups and key informant interviews. Spearhead special projects, including the design, implementation, and analysis of key surveys such as the First 5 Kern Developmental Screening Gap Assessment and the Parent/Guardian Survey and Vaccination and Immunization for the Kery County Immunization Coalition.</t>
+  </si>
+  <si>
+    <t>Serve as Lead Project Manager for ASR's consulting work with three California County Offices of Education. Oversee the design and execution of Needs Assessments and parent surveys focused on perceptions, barriers, and priorities related to child care availability, priorities, and barriers to access.</t>
+  </si>
+  <si>
+    <t>https://jim-asr.shinyapps.io/SantaCruz_UPK_Survey/</t>
+  </si>
+  <si>
+    <t>https://jim-asr.shinyapps.io/KernCountyImmunizationCoalition_SurveyResults/</t>
   </si>
 </sst>
 </file>
@@ -767,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8559F42B-99AA-F44B-B1DC-6C413C767572}">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -869,7 +887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1505,27 +1523,27 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B42" s="1">
-        <v>2023</v>
-      </c>
-      <c r="C42" s="1">
         <v>2024</v>
       </c>
+      <c r="C42" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D42" s="1" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>95</v>
+        <v>124</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -1533,25 +1551,25 @@
         <v>86</v>
       </c>
       <c r="B43" s="1">
-        <v>2023</v>
-      </c>
-      <c r="C43" s="1">
         <v>2024</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="D43" s="1" t="s">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="255" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>86</v>
       </c>
@@ -1562,19 +1580,16 @@
         <v>2024</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="238" x14ac:dyDescent="0.2">
@@ -1582,54 +1597,51 @@
         <v>86</v>
       </c>
       <c r="B45" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C45" s="1">
         <v>2024</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="153" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="255" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B46" s="1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C46" s="1">
         <v>2024</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="289" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="238" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
@@ -1640,48 +1652,48 @@
         <v>2024</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="187" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="153" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="B48" s="1">
         <v>2022</v>
       </c>
       <c r="C48" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="323" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="289" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>86</v>
       </c>
@@ -1689,24 +1701,27 @@
         <v>2022</v>
       </c>
       <c r="C49" s="1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="187" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B50" s="1">
         <v>2022</v>
@@ -1715,15 +1730,64 @@
         <v>2023</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F50" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="323" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C51" s="1">
+        <v>2023</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="102" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2022</v>
+      </c>
+      <c r="C52" s="1">
+        <v>2023</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F52" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="I52" s="1" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>